<commit_message>
Revert "Add some changes on fe"
This reverts commit 17f2ce3fbc04e4c4bdd6bd10983d941cf9c2d408.
</commit_message>
<xml_diff>
--- a/Document/Sprint Info/Sprint3_Info_Team1.xlsx
+++ b/Document/Sprint Info/Sprint3_Info_Team1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FPTU_References\chuyenNganh6\OJT\Sprint3\Sprint Info\Document\Sprint Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FPTU_References\chuyenNganh6\OJT\Sprint3\group1\Document\Sprint Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74962D-3ECD-4676-AB04-F03D0A3FA6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE32715D-F9FD-466F-A718-1B7A3D234ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Info" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>BE</t>
   </si>
   <si>
-    <t>Process</t>
-  </si>
-  <si>
     <t>DuyNM</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>Write API for Update Certificate of Course</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -730,13 +730,13 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,39 +1056,39 @@
   </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="69.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1112,7 +1112,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="10" t="s">
         <v>6</v>
@@ -1140,7 +1140,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="10" t="s">
         <v>9</v>
@@ -1168,7 +1168,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="13" t="s">
         <v>12</v>
@@ -1194,7 +1194,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="17" t="s">
         <v>14</v>
@@ -1224,7 +1224,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="17" t="s">
         <v>9</v>
@@ -1254,7 +1254,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="20" t="s">
         <v>17</v>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="12">
         <v>0</v>
@@ -1284,14 +1284,14 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="12">
         <v>0</v>
@@ -1308,14 +1308,14 @@
       <c r="M9" s="16"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="23"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="12">
         <v>0</v>
@@ -1332,14 +1332,14 @@
       <c r="M10" s="16"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="23"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="12">
         <v>0</v>
@@ -1356,14 +1356,14 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="23"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="12">
         <v>0</v>
@@ -1380,7 +1380,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="23"/>
@@ -1404,7 +1404,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1420,7 +1420,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1436,7 +1436,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1447,7 +1447,7 @@
         <v>19</v>
       </c>
       <c r="H16" s="26"/>
-      <c r="I16" s="48">
+      <c r="I16" s="46">
         <f>SUM(I18:I48)</f>
         <v>95.5</v>
       </c>
@@ -1457,7 +1457,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>20</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>1</v>
       </c>
@@ -1499,19 +1499,19 @@
         <v>27</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="32">
         <v>3</v>
       </c>
       <c r="F18" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>30</v>
       </c>
       <c r="H18" s="33">
         <v>45478</v>
@@ -1525,7 +1525,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30">
         <v>2</v>
       </c>
@@ -1533,16 +1533,16 @@
         <v>27</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="32">
         <v>3</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G19" s="31" t="s">
         <v>8</v>
@@ -1559,7 +1559,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30">
         <v>3</v>
       </c>
@@ -1567,16 +1567,16 @@
         <v>27</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="32">
         <v>3</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>16</v>
@@ -1593,7 +1593,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30">
         <v>4</v>
       </c>
@@ -1601,19 +1601,19 @@
         <v>27</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="32">
         <v>3</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="33">
         <v>45478</v>
@@ -1627,7 +1627,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30">
         <v>5</v>
       </c>
@@ -1635,19 +1635,19 @@
         <v>27</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="32">
         <v>3</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H22" s="33">
         <v>45478</v>
@@ -1661,7 +1661,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30">
         <v>6</v>
       </c>
@@ -1669,16 +1669,16 @@
         <v>27</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="32">
         <v>3</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G23" s="27" t="s">
         <v>11</v>
@@ -1695,7 +1695,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30">
         <v>7</v>
       </c>
@@ -1703,16 +1703,16 @@
         <v>27</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="32">
         <v>3</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G24" s="27" t="s">
         <v>15</v>
@@ -1729,7 +1729,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
         <v>8</v>
       </c>
@@ -1737,19 +1737,19 @@
         <v>27</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="32">
         <v>3</v>
       </c>
       <c r="F25" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>30</v>
       </c>
       <c r="H25" s="33">
         <v>45478</v>
@@ -1763,7 +1763,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30">
         <v>9</v>
       </c>
@@ -1771,16 +1771,16 @@
         <v>27</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="32">
         <v>3</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G26" s="31" t="s">
         <v>8</v>
@@ -1797,7 +1797,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30">
         <v>10</v>
       </c>
@@ -1805,16 +1805,16 @@
         <v>27</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="32">
         <v>3</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G27" s="31" t="s">
         <v>16</v>
@@ -1831,7 +1831,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30">
         <v>11</v>
       </c>
@@ -1839,19 +1839,19 @@
         <v>27</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="32">
         <v>3</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H28" s="33">
         <v>45478</v>
@@ -1865,7 +1865,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30">
         <v>12</v>
       </c>
@@ -1873,19 +1873,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="32">
         <v>3</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H29" s="33">
         <v>45478</v>
@@ -1899,7 +1899,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30">
         <v>13</v>
       </c>
@@ -1907,19 +1907,19 @@
         <v>28</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="32">
         <v>3</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" s="33">
         <v>45478</v>
@@ -1933,7 +1933,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30">
         <v>14</v>
       </c>
@@ -1941,19 +1941,19 @@
         <v>28</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="32">
         <v>3</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H31" s="33">
         <v>45478</v>
@@ -1967,7 +1967,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30">
         <v>15</v>
       </c>
@@ -1975,16 +1975,16 @@
         <v>28</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="32">
         <v>3</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G32" s="27" t="s">
         <v>13</v>
@@ -2001,7 +2001,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30">
         <v>16</v>
       </c>
@@ -2009,19 +2009,19 @@
         <v>28</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="32">
         <v>3</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="33">
         <v>45478</v>
@@ -2035,7 +2035,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30">
         <v>17</v>
       </c>
@@ -2043,19 +2043,19 @@
         <v>28</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="32">
         <v>3</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H34" s="33">
         <v>45478</v>
@@ -2069,7 +2069,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="30">
         <v>18</v>
       </c>
@@ -2077,16 +2077,16 @@
         <v>28</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" s="32">
         <v>3</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G35" s="27" t="s">
         <v>13</v>
@@ -2103,7 +2103,7 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>19</v>
       </c>
@@ -2111,19 +2111,19 @@
         <v>28</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="32">
         <v>3</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H36" s="33">
         <v>45478</v>
@@ -2132,7 +2132,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>20</v>
       </c>
@@ -2140,19 +2140,19 @@
         <v>28</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="32">
         <v>3</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H37" s="33">
         <v>45478</v>
@@ -2161,7 +2161,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>21</v>
       </c>
@@ -2169,16 +2169,16 @@
         <v>28</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="32">
         <v>3</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G38" s="27" t="s">
         <v>13</v>
@@ -2190,7 +2190,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>22</v>
       </c>
@@ -2198,19 +2198,19 @@
         <v>28</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="32">
         <v>3</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H39" s="33">
         <v>45478</v>
@@ -2219,7 +2219,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>23</v>
       </c>
@@ -2227,19 +2227,19 @@
         <v>28</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" s="32">
         <v>3</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H40" s="33">
         <v>45478</v>
@@ -2248,7 +2248,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>24</v>
       </c>
@@ -2256,16 +2256,16 @@
         <v>28</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E41" s="32">
         <v>3</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G41" s="27" t="s">
         <v>13</v>
@@ -2277,7 +2277,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>25</v>
       </c>
@@ -2285,19 +2285,19 @@
         <v>28</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="32">
         <v>3</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H42" s="33">
         <v>45478</v>
@@ -2306,7 +2306,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>26</v>
       </c>
@@ -2314,19 +2314,19 @@
         <v>28</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43" s="32">
         <v>3</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H43" s="33">
         <v>45478</v>
@@ -2335,7 +2335,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>27</v>
       </c>
@@ -2343,16 +2343,16 @@
         <v>28</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44" s="32">
         <v>3</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G44" s="27" t="s">
         <v>13</v>
@@ -2364,7 +2364,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>28</v>
       </c>
@@ -2372,19 +2372,19 @@
         <v>28</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45" s="32">
         <v>3</v>
       </c>
       <c r="F45" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H45" s="33">
         <v>45478</v>
@@ -2393,7 +2393,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>29</v>
       </c>
@@ -2401,19 +2401,19 @@
         <v>28</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46" s="32">
         <v>3</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H46" s="33">
         <v>45478</v>
@@ -2422,7 +2422,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>30</v>
       </c>
@@ -2430,16 +2430,16 @@
         <v>28</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" s="32">
         <v>3</v>
       </c>
       <c r="F47" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G47" s="27" t="s">
         <v>13</v>
@@ -2451,7 +2451,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>31</v>
       </c>
@@ -2459,19 +2459,19 @@
         <v>28</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E48" s="32">
         <v>3</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H48" s="33">
         <v>45478</v>

</xml_diff>